<commit_message>
Corrige grilla en x e y
</commit_message>
<xml_diff>
--- a/Modelo/grillas.xlsx
+++ b/Modelo/grillas.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2DFD298E-C334-47F1-8953-0742105C40C3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -18,8 +19,25 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+  <si>
+    <t>dist</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>11'</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -29,12 +47,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -49,8 +73,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +358,273 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12:D21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <f>C2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1.36</v>
+      </c>
+      <c r="D3">
+        <f>D2+C3</f>
+        <v>1.36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>2.41</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D21" si="0">D3+C4</f>
+        <v>3.7700000000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>2.73</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>1.2</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>1.4</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>1.6</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>1.84</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>12.54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>3.76</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>16.299999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>0.54</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>16.839999999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>2.9</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>19.739999999999995</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="2">
+        <v>11</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1.84</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="shared" si="0"/>
+        <v>21.579999999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>0.16</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>21.739999999999995</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>12</v>
+      </c>
+      <c r="C15">
+        <v>1.6</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>23.339999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <v>13</v>
+      </c>
+      <c r="C16">
+        <v>1.4</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>24.739999999999995</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="2">
+        <v>14</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" si="0"/>
+        <v>25.939999999999994</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>15</v>
+      </c>
+      <c r="C18">
+        <v>2.65</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>28.589999999999993</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>16</v>
+      </c>
+      <c r="C19">
+        <v>2.64</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>31.229999999999993</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>17</v>
+      </c>
+      <c r="C20">
+        <v>1.04</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>32.269999999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>18</v>
+      </c>
+      <c r="C21">
+        <v>7.01</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>39.279999999999994</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>